<commit_message>
updates to prioritization report; adding recommended actions excel file
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20240410.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20240410.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E9569-E138-420D-8EDA-92666375D94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48C633A-88A6-47A5-B88A-E747059076BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" tabRatio="581" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3639" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3639" uniqueCount="906">
   <si>
     <t>stream</t>
   </si>
@@ -3071,6 +3071,9 @@
   </si>
   <si>
     <t>WR1 should continue to be funded under the project. A two-pass array at MR1 would allow an estimate of a detection probability at both WR1 and the lower array and MR1 and allow parsing of abundance among steelhead major spawning areas and sp/sum Chinook populations. However, estimates of detection probabilities at WR1 have been found to be biased due to Minam and Wallowa adults "sorting" by the time they arrive to WR1. Therefore, a single-pass array at WR2 should also be funded under the project to ensure unbiased detection probability estimates.</t>
+  </si>
+  <si>
+    <t>Add IPTDS (2)</t>
   </si>
 </sst>
 </file>
@@ -4720,13 +4723,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI104"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="C100" sqref="C19:C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4875,7 +4879,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>95</v>
       </c>
@@ -4973,7 +4977,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
@@ -5071,7 +5075,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
@@ -5169,7 +5173,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -5265,7 +5269,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>99</v>
       </c>
@@ -5363,7 +5367,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>231</v>
       </c>
@@ -5449,7 +5453,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>41</v>
       </c>
@@ -5547,7 +5551,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>42</v>
       </c>
@@ -5645,7 +5649,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
@@ -5743,7 +5747,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>43</v>
       </c>
@@ -5841,7 +5845,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>45</v>
       </c>
@@ -5941,7 +5945,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
@@ -6039,7 +6043,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>47</v>
       </c>
@@ -6141,7 +6145,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>48</v>
       </c>
@@ -6241,7 +6245,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>50</v>
       </c>
@@ -6341,7 +6345,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>49</v>
       </c>
@@ -6439,7 +6443,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
         <v>51</v>
       </c>
@@ -6737,7 +6741,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>856</v>
       </c>
@@ -6831,7 +6835,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>272</v>
       </c>
@@ -6917,7 +6921,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>276</v>
       </c>
@@ -7203,7 +7207,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>52</v>
       </c>
@@ -7501,7 +7505,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>57</v>
       </c>
@@ -7601,7 +7605,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>58</v>
       </c>
@@ -7701,7 +7705,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>61</v>
       </c>
@@ -7801,7 +7805,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>62</v>
       </c>
@@ -8001,7 +8005,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>91</v>
       </c>
@@ -8101,7 +8105,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>92</v>
       </c>
@@ -8201,7 +8205,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
         <v>93</v>
       </c>
@@ -8301,7 +8305,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
         <v>94</v>
       </c>
@@ -8499,7 +8503,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>65</v>
       </c>
@@ -8701,7 +8705,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
         <v>71</v>
       </c>
@@ -8803,7 +8807,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
         <v>72</v>
       </c>
@@ -8905,7 +8909,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>865</v>
       </c>
@@ -9093,7 +9097,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>68</v>
       </c>
@@ -9193,7 +9197,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>67</v>
       </c>
@@ -9295,7 +9299,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>69</v>
       </c>
@@ -9397,7 +9401,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>119</v>
       </c>
@@ -9789,7 +9793,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
         <v>89</v>
       </c>
@@ -10085,7 +10089,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>367</v>
       </c>
@@ -10269,7 +10273,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>121</v>
       </c>
@@ -10471,7 +10475,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>100</v>
       </c>
@@ -10669,7 +10673,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>104</v>
       </c>
@@ -10769,7 +10773,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="17" t="s">
         <v>387</v>
       </c>
@@ -10855,7 +10859,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="17" t="s">
         <v>390</v>
       </c>
@@ -10941,7 +10945,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
         <v>394</v>
       </c>
@@ -11127,7 +11131,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
         <v>400</v>
       </c>
@@ -11211,7 +11215,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
         <v>105</v>
       </c>
@@ -11311,7 +11315,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
         <v>107</v>
       </c>
@@ -11409,7 +11413,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
         <v>108</v>
       </c>
@@ -11509,7 +11513,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
         <v>109</v>
       </c>
@@ -11607,7 +11611,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
         <v>416</v>
       </c>
@@ -11993,7 +11997,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>111</v>
       </c>
@@ -12091,7 +12095,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>112</v>
       </c>
@@ -12191,7 +12195,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>113</v>
       </c>
@@ -12289,7 +12293,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
         <v>437</v>
       </c>
@@ -12473,7 +12477,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>115</v>
       </c>
@@ -12571,7 +12575,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>116</v>
       </c>
@@ -12769,7 +12773,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>118</v>
       </c>
@@ -12869,7 +12873,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>454</v>
       </c>
@@ -13151,7 +13155,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="17" t="s">
         <v>124</v>
       </c>
@@ -13253,7 +13257,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
         <v>467</v>
       </c>
@@ -13435,7 +13439,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="17" t="s">
         <v>126</v>
       </c>
@@ -13533,7 +13537,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="17" t="s">
         <v>127</v>
       </c>
@@ -13633,7 +13637,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>861</v>
       </c>
@@ -13819,7 +13823,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="17" t="s">
         <v>82</v>
       </c>
@@ -14119,7 +14123,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="17" t="s">
         <v>76</v>
       </c>
@@ -14219,7 +14223,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="17" t="s">
         <v>491</v>
       </c>
@@ -14505,7 +14509,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="17" t="s">
         <v>79</v>
       </c>
@@ -14605,7 +14609,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="17" t="s">
         <v>80</v>
       </c>
@@ -14705,7 +14709,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="17" t="s">
         <v>81</v>
       </c>
@@ -14807,7 +14811,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="17" t="s">
         <v>83</v>
       </c>
@@ -14910,6 +14914,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI104" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -18256,7 +18267,7 @@
   <dimension ref="B1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18363,7 +18374,7 @@
         <v>761</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>876</v>
+        <v>905</v>
       </c>
       <c r="H6" s="59" t="s">
         <v>891</v>

</xml_diff>